<commit_message>
Added ability to be used as a clock generator.
</commit_message>
<xml_diff>
--- a/PCB/harp expander BOM.xlsx
+++ b/PCB/harp expander BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Google Drive\projects\harp-tech\harp expander v1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562D35F5-BC1A-4580-BD91-2B6CB892B74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4C939-3C9B-4275-9C59-188A579DD65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="120">
   <si>
     <t>Qty</t>
   </si>
@@ -66,9 +66,6 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>C1, C3, C5, C7, C9, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C25, C26, C27, C28, C29, C30, C31, C32</t>
-  </si>
-  <si>
     <t>MC0402B104K160CT</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>CRCW040210R0FKEDHP</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R53</t>
-  </si>
-  <si>
     <t>CRCW04021K00FKED</t>
   </si>
   <si>
@@ -207,18 +198,6 @@
     <t>73100-0105</t>
   </si>
   <si>
-    <t>CLCK Jumper</t>
-  </si>
-  <si>
-    <t>JP2</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>42375-1856</t>
-  </si>
-  <si>
     <t>CLCK_JACK</t>
   </si>
   <si>
@@ -291,9 +270,6 @@
     <t>SOT23-5</t>
   </si>
   <si>
-    <t>IC7, IC14</t>
-  </si>
-  <si>
     <t>TLV70033DDCR</t>
   </si>
   <si>
@@ -363,9 +339,6 @@
     <t>USB2HABM3RA</t>
   </si>
   <si>
-    <t>R3, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R38, R43, R46, R47</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -403,6 +376,21 @@
   </si>
   <si>
     <t>TH</t>
+  </si>
+  <si>
+    <t>IC7, IC8, IC9, IC10</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C7, C9, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C25, C26, C27, C28, C29, C30, C31, C32, C35, C36</t>
+  </si>
+  <si>
+    <t>R3, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R38, R43, R46, R47, R54, R55</t>
+  </si>
+  <si>
+    <t>R2, R53</t>
+  </si>
+  <si>
+    <t>R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31</t>
   </si>
 </sst>
 </file>
@@ -1300,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1321,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1353,12 +1341,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1367,53 +1355,53 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1421,39 +1409,39 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1461,19 +1449,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,19 +1469,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1501,19 +1489,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1521,19 +1509,19 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,19 +1529,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1561,19 +1549,19 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,16 +1569,16 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1598,19 +1586,19 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1618,19 +1606,19 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1638,53 +1626,53 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,19 +1680,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" t="s">
-        <v>68</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1712,19 +1700,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
         <v>69</v>
       </c>
-      <c r="C21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1732,19 +1720,19 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1752,39 +1740,39 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,39 +1780,39 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1832,19 +1820,19 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,36 +1840,24 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1889,7 +1865,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,109 +1873,97 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>105</v>
-      </c>
-      <c r="E39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F41" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F42" s="1">
-        <v>116</v>
-      </c>
-      <c r="G42">
-        <f>130-14</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections to BOMs.
</commit_message>
<xml_diff>
--- a/PCB/harp expander BOM.xlsx
+++ b/PCB/harp expander BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED1270B-153F-4758-B03E-01F17CBEE96D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1172DE9F-E44D-45B8-B99E-131877BC1B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1326,7 +1326,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed the audio cable PN.
</commit_message>
<xml_diff>
--- a/PCB/harp expander BOM.xlsx
+++ b/PCB/harp expander BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Google Drive\projects\harp-tech\harp_expander\harp expander v1.0 READY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2AD0CF-44CB-4020-B1D6-208D2A718564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB371B-0FE1-48A2-B399-AAF2573426CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,9 +318,6 @@
     <t>HEADER_3x2</t>
   </si>
   <si>
-    <t>3.5mm stereo jack cable 0.3 m, Black</t>
-  </si>
-  <si>
     <t>0.9 left angle USB cable</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>PCB COMPONENTS</t>
+  </si>
+  <si>
+    <t>3.5mm stereo jack cable 1.2 m, Black</t>
   </si>
 </sst>
 </file>
@@ -1313,9 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1344,12 +1342,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1374,7 +1372,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1388,13 +1386,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1408,13 +1406,13 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1428,13 +1426,13 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1454,7 +1452,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1468,13 +1466,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1514,7 +1512,7 @@
         <v>92</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1534,7 +1532,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,7 +1552,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1574,7 +1572,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,7 +1592,7 @@
         <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1611,7 +1609,7 @@
         <v>43</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1631,7 +1629,7 @@
         <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1651,7 +1649,7 @@
         <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1668,7 +1666,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1685,7 +1683,7 @@
         <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,7 +1703,7 @@
         <v>61</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,7 +1723,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1745,7 +1743,7 @@
         <v>69</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1765,7 +1763,7 @@
         <v>72</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1785,7 +1783,7 @@
         <v>76</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1799,13 +1797,13 @@
         <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
         <v>77</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,7 +1823,7 @@
         <v>79</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,7 +1843,7 @@
         <v>82</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,7 +1863,7 @@
         <v>88</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,7 +1880,7 @@
         <v>91</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1890,12 +1888,12 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1908,10 +1906,10 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1930,10 +1928,10 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" t="s">
         <v>101</v>
-      </c>
-      <c r="E34" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1941,15 +1939,15 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1962,10 +1960,10 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1973,15 +1971,15 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1991,7 +1989,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F40" s="1">
         <v>27</v>
@@ -1999,7 +1997,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" s="1">
         <v>122</v>
@@ -2007,7 +2005,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F42" s="1">
         <v>13</v>

</xml_diff>

<commit_message>
Replaced oscillator with a more precise one.
</commit_message>
<xml_diff>
--- a/PCB/harp expander BOM.xlsx
+++ b/PCB/harp expander BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Google Drive\projects\harp-tech\harp_expander\harp expander v1.0 READY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB371B-0FE1-48A2-B399-AAF2573426CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D3D91D-7B61-421A-AF05-71226CF5D0E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>Qty</t>
   </si>
@@ -243,9 +243,6 @@
     <t>OSC</t>
   </si>
   <si>
-    <t>DSC1001CI5-032.0000T</t>
-  </si>
-  <si>
     <t>PROG HEADER</t>
   </si>
   <si>
@@ -397,6 +394,12 @@
   </si>
   <si>
     <t>3.5mm stereo jack cable 1.2 m, Black</t>
+  </si>
+  <si>
+    <t>O 32,0-JT32C-A-K-3,3-LF</t>
+  </si>
+  <si>
+    <t>Alternative: DSC1001CI5-032.0000T</t>
   </si>
 </sst>
 </file>
@@ -928,7 +931,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -943,6 +946,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1311,9 +1317,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1323,6 +1331,7 @@
     <col min="4" max="4" width="97.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1342,18 +1351,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1372,7 +1381,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,13 +1395,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1406,13 +1415,13 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,13 +1435,13 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,7 +1461,7 @@
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1466,13 +1475,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,7 +1501,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1508,11 +1517,11 @@
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
-        <v>92</v>
+      <c r="E10" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,7 +1541,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,7 +1561,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,7 +1581,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,7 +1601,7 @@
         <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1609,7 +1618,7 @@
         <v>43</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1629,10 +1638,10 @@
         <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>12</v>
       </c>
@@ -1649,10 +1658,10 @@
         <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>5</v>
       </c>
@@ -1666,10 +1675,10 @@
         <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>2</v>
       </c>
@@ -1683,10 +1692,10 @@
         <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -1703,10 +1712,10 @@
         <v>61</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>1</v>
       </c>
@@ -1723,10 +1732,10 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>1</v>
       </c>
@@ -1739,177 +1748,180 @@
       <c r="D22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
-        <v>69</v>
+      <c r="E22" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>71</v>
       </c>
-      <c r="E23" t="s">
-        <v>72</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>74</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>75</v>
       </c>
-      <c r="E24" t="s">
-        <v>76</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>4</v>
       </c>
       <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>77</v>
       </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
         <v>79</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>80</v>
       </c>
-      <c r="D26" t="s">
-        <v>81</v>
-      </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>83</v>
       </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
       <c r="E27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
         <v>85</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>86</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>87</v>
       </c>
-      <c r="E28" t="s">
-        <v>88</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
         <v>89</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>90</v>
       </c>
-      <c r="E29" t="s">
-        <v>91</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,10 +1929,10 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
         <v>100</v>
-      </c>
-      <c r="E34" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1939,31 +1951,31 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="A36" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,25 +1983,25 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="A39" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F40" s="1">
         <v>27</v>
@@ -1997,7 +2009,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F41" s="1">
         <v>122</v>
@@ -2005,7 +2017,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F42" s="1">
         <v>13</v>

</xml_diff>

<commit_message>
Added filtering on inputs and reset lines to prevent erroneous behavior in noisy environments.
</commit_message>
<xml_diff>
--- a/PCB/harp expander BOM.xlsx
+++ b/PCB/harp expander BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3F739A-CBF0-402B-85F6-4411A034160B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93140D3F-DC33-4BA0-86C4-09D81D2537CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'harp expander v1'!$A$32:$F$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'harp expander v1'!$A$33:$F$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
   <si>
     <t>Qty</t>
   </si>
@@ -57,9 +57,6 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R4, R5, R6, R7, R8, R48, R49, R50, R51, R52</t>
-  </si>
-  <si>
     <t>CRCW0603100RFKEAHP</t>
   </si>
   <si>
@@ -87,15 +84,6 @@
     <t>CRCW040210K0FKED</t>
   </si>
   <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>CRCW04021M00FKED</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -123,21 +111,9 @@
     <t>C0603</t>
   </si>
   <si>
-    <t>C10, C11, C23, C24, C33, C34, C37, C38</t>
-  </si>
-  <si>
     <t>C1608X6S1C475K080AC</t>
   </si>
   <si>
-    <t>A/3216-18W</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>TAJA475K016UNJ</t>
-  </si>
-  <si>
     <t>40R@100MHz</t>
   </si>
   <si>
@@ -159,9 +135,6 @@
     <t>04025A470JAT2A</t>
   </si>
   <si>
-    <t>569-0112-100</t>
-  </si>
-  <si>
     <t>LED0, LED1, LED2, LED3, LED4, LED5</t>
   </si>
   <si>
@@ -312,9 +285,6 @@
     <t>885012205084</t>
   </si>
   <si>
-    <t>HEADER_3x2</t>
-  </si>
-  <si>
     <t>0.9 left angle USB cable</t>
   </si>
   <si>
@@ -366,15 +336,6 @@
     <t>IC7, IC8, IC9, IC10</t>
   </si>
   <si>
-    <t>C1, C3, C5, C7, C9, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C25, C26, C27, C28, C29, C30, C31, C32, C35, C36</t>
-  </si>
-  <si>
-    <t>R3, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R38, R43, R46, R47, R54, R55</t>
-  </si>
-  <si>
-    <t>R2, R53</t>
-  </si>
-  <si>
     <t>R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31</t>
   </si>
   <si>
@@ -400,6 +361,72 @@
   </si>
   <si>
     <t>Alternative: DSC1001CI5-032.0000T</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C7, C9, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C25, C26, C27, C28, C29, C30, C31, C32, C35, C36, C40</t>
+  </si>
+  <si>
+    <t>C10, C11, C23, C24, C33, C34, C37, C38, C52</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3, R9, R10, R11, R12, R13, R14, R15, R16, R17, R19, R38, R43, R46, R47, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68</t>
+  </si>
+  <si>
+    <t>R4, R5, R6, R7, R8, R48, R49, R50, R51, R52, R69</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>TT2D6</t>
+  </si>
+  <si>
+    <t>569-011X-X00_LED_ARRAY</t>
+  </si>
+  <si>
+    <t>MA03-2</t>
+  </si>
+  <si>
+    <t>SO14</t>
+  </si>
+  <si>
+    <t>240-0002-1</t>
+  </si>
+  <si>
+    <t>EEUFM1E101B</t>
+  </si>
+  <si>
+    <t>C0402C331J5GACTU</t>
+  </si>
+  <si>
+    <t>74HCT125D,653</t>
+  </si>
+  <si>
+    <t>100u 25V</t>
+  </si>
+  <si>
+    <t>330pF</t>
+  </si>
+  <si>
+    <t>RED_LEDs</t>
+  </si>
+  <si>
+    <t>74HCT125SO14</t>
+  </si>
+  <si>
+    <t>Number of unique SMD parts</t>
+  </si>
+  <si>
+    <t>Number of unique TH parts</t>
   </si>
 </sst>
 </file>
@@ -759,7 +786,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -874,6 +901,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -931,7 +967,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -940,17 +976,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1317,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,8 +1365,8 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="97.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="4" max="4" width="130.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1351,97 +1388,94 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1449,490 +1483,511 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="F19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D28" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="E28" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="F28" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>88</v>
-      </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
       <c r="D30" t="s">
-        <v>96</v>
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" t="s">
-        <v>114</v>
-      </c>
+      <c r="A32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1940,95 +1995,122 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" t="s">
-        <v>94</v>
-      </c>
+      <c r="A37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
       <c r="D38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F41" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F42" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F40" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F41" s="1">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>104</v>
-      </c>
-      <c r="F42" s="1">
-        <v>13</v>
+      <c r="F44" s="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="1">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>